<commit_message>
added group logs and stealing behaviour
</commit_message>
<xml_diff>
--- a/Genetics2020.xlsx
+++ b/Genetics2020.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\KamGenetics2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3DE007-F410-44AF-8F4D-48E6C3A59EE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF3115A-58D2-4950-AF64-8DD736512B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Obtain Resource" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>Economy/Military</t>
   </si>
@@ -88,13 +94,34 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Individual Steal</t>
+  </si>
+  <si>
+    <t>Military Preparedness</t>
+  </si>
+  <si>
+    <t>Attacker</t>
+  </si>
+  <si>
+    <t>Defender</t>
+  </si>
+  <si>
+    <t>% Success</t>
+  </si>
+  <si>
+    <t>Willing to kill</t>
+  </si>
+  <si>
+    <t>+20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,8 +135,14 @@
       <name val="Hack"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Hack"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,8 +159,19 @@
         <fgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -135,20 +179,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" customWidth="1"/>
     <col min="4" max="5" width="36.7109375" customWidth="1"/>
@@ -649,6 +729,48 @@
         <v>15</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <f>MAX(0,A24-B24+$C$23)</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>